<commit_message>
updates from sanaa pc
</commit_message>
<xml_diff>
--- a/uncertainty_models/UMCPVF_I1.xlsx
+++ b/uncertainty_models/UMCPVF_I1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\uncertainty_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26994C0-5C94-4573-AEBA-95A4F5BEE22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BC2EF9-A1EA-492C-8007-60DD0E90CB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="001" sheetId="1" r:id="rId1"/>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3523,8 +3523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3768,10 +3768,10 @@
         <v>27</v>
       </c>
       <c r="B4" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="C4" s="18">
-        <v>0.05</v>
+        <v>0</v>
+      </c>
+      <c r="C4" s="17">
+        <v>0</v>
       </c>
       <c r="D4" s="17">
         <v>0.1</v>
@@ -3845,10 +3845,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="18">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0</v>
       </c>
       <c r="D5" s="17">
         <v>0.5</v>

</xml_diff>

<commit_message>
template and initial data with 0 stocks
</commit_message>
<xml_diff>
--- a/uncertainty_models/UMCPVF_I1.xlsx
+++ b/uncertainty_models/UMCPVF_I1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\uncertainty_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9A3A3A-C27D-455C-A4BB-42A75002F542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4D5CED-D1BE-441F-BBDF-4100EFBF390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3015" yWindow="690" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="001" sheetId="1" r:id="rId1"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -700,70 +700,70 @@
         <v>0</v>
       </c>
       <c r="D2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="E2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="F2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="G2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="H2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="I2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="J2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="K2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="L2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="M2" s="9">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="N2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="O2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="P2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="Q2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="R2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="S2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="T2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="U2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="V2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="W2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="X2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="Y2" s="10">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -777,70 +777,70 @@
         <v>0</v>
       </c>
       <c r="D3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="E3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="F3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="G3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="H3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="I3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="J3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="L3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="M3" s="9">
-        <v>-0.5</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="N3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="O3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="P3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="Q3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="R3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="S3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="T3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="U3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="V3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="W3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="X3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="Y3" s="10">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -2064,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2191,40 +2191,40 @@
         <v>0</v>
       </c>
       <c r="N2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="O2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="P2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="Q2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="R2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="S2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="T2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="U2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="V2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="W2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="X2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
       <c r="Y2" s="15">
-        <v>-0.5</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2268,40 +2268,40 @@
         <v>0</v>
       </c>
       <c r="N3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="O3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="P3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="Q3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="R3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="S3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="T3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="U3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="V3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="W3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="X3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="Y3" s="15">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -2315,70 +2315,70 @@
         <v>0</v>
       </c>
       <c r="D4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="I4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M4" s="12">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="O4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="P4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="Q4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="R4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="S4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="T4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="U4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="V4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="W4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="X4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="Y4" s="15">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -2392,70 +2392,70 @@
         <v>0</v>
       </c>
       <c r="D5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="G5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="H5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="I5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="J5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="K5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="L5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="M5" s="12">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="N5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="O5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="P5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="Q5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="R5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="S5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="T5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="U5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="V5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="W5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="X5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="Y5" s="15">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -3525,8 +3525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3652,40 +3652,40 @@
         <v>0</v>
       </c>
       <c r="N2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="O2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="P2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="Q2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="R2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="S2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="T2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="U2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="V2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="W2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="X2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="Y2" s="20">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -3729,40 +3729,40 @@
         <v>0</v>
       </c>
       <c r="N3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="O3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="P3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="Q3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="R3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="S3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="T3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="U3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="V3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="W3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="X3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="Y3" s="20">
-        <v>-0.05</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -3776,70 +3776,70 @@
         <v>0</v>
       </c>
       <c r="D4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="G4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="H4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="I4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="J4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="K4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="L4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="M4" s="17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="N4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="Q4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="R4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="S4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="T4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="U4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="V4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="W4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="X4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="Y4" s="20">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -3853,70 +3853,70 @@
         <v>0</v>
       </c>
       <c r="D5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="L5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M5" s="17">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="N5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="O5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="P5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="Q5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="R5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="S5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="T5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="U5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="V5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="W5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="X5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="Y5" s="20">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -4987,7 +4987,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>